<commit_message>
Various December 2 Changes
</commit_message>
<xml_diff>
--- a/sub_pro_11_kcpe_kcse/processed_tables/kcse_1.xlsx
+++ b/sub_pro_11_kcpe_kcse/processed_tables/kcse_1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\R_Files\afrodataviz\sub_pro_11_kcpe_kcse\processed_tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5FE8BF3-765F-430E-AC57-7BC37C042AF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF9DDCF8-DFD2-4133-AF23-E286DEC4529F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2460" windowWidth="19200" windowHeight="7360" xr2:uid="{BE84807C-8315-435C-B8E2-3CA01EE3DA82}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="18590" windowHeight="10420" xr2:uid="{BE84807C-8315-435C-B8E2-3CA01EE3DA82}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="21">
   <si>
     <t>Year</t>
   </si>
@@ -70,6 +70,24 @@
   </si>
   <si>
     <t>Total (C-E)</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>C-</t>
+  </si>
+  <si>
+    <t>D+</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>D-</t>
+  </si>
+  <si>
+    <t>E</t>
   </si>
 </sst>
 </file>
@@ -428,10 +446,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57EF4774-BC58-4EE6-8DB6-E5825ED7B550}">
-  <dimension ref="A1:AZ12"/>
+  <dimension ref="A1:AZ19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1748,788 +1766,1792 @@
     </row>
     <row r="9" spans="1:52" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9">
-        <f>SUM(B3:B8)</f>
-        <v>38248</v>
-      </c>
-      <c r="C9">
-        <f>SUM(C3:C8)</f>
-        <v>24856</v>
+        <v>15</v>
+      </c>
+      <c r="B9" s="3">
+        <v>16450</v>
+      </c>
+      <c r="C9" s="3">
+        <v>14212</v>
       </c>
       <c r="D9">
-        <f>SUM(D3:D8)</f>
-        <v>63104</v>
-      </c>
-      <c r="E9">
-        <f>SUM(E3:E8)</f>
-        <v>51261</v>
-      </c>
-      <c r="F9">
-        <f>SUM(F3:F8)</f>
-        <v>30873</v>
+        <f t="shared" ref="D9:D14" si="7">SUM(B9:C9)</f>
+        <v>30662</v>
+      </c>
+      <c r="E9" s="3">
+        <v>19847</v>
+      </c>
+      <c r="F9" s="3">
+        <v>16981</v>
       </c>
       <c r="G9">
-        <f>SUM(G3:G8)</f>
-        <v>82134</v>
-      </c>
-      <c r="H9">
-        <f>SUM(H3:H8)</f>
-        <v>44310</v>
-      </c>
-      <c r="I9">
-        <f>SUM(I3:I8)</f>
-        <v>28339</v>
+        <f t="shared" ref="G9:G14" si="8">SUM(E9:F9)</f>
+        <v>36828</v>
+      </c>
+      <c r="H9" s="3">
+        <v>18763</v>
+      </c>
+      <c r="I9" s="3">
+        <v>15357</v>
       </c>
       <c r="J9">
-        <f>SUM(J3:J8)</f>
-        <v>72649</v>
-      </c>
-      <c r="K9">
-        <f>SUM(K3:K8)</f>
-        <v>50109</v>
-      </c>
-      <c r="L9">
-        <f>SUM(L3:L8)</f>
-        <v>30939</v>
+        <f t="shared" ref="J9:J14" si="9">SUM(H9:I9)</f>
+        <v>34120</v>
+      </c>
+      <c r="K9" s="3">
+        <v>22327</v>
+      </c>
+      <c r="L9" s="3">
+        <v>17418</v>
       </c>
       <c r="M9">
-        <f>SUM(M3:M8)</f>
-        <v>81048</v>
-      </c>
-      <c r="N9">
-        <f>SUM(N3:N8)</f>
-        <v>60200</v>
-      </c>
-      <c r="O9">
-        <f>SUM(O3:O8)</f>
-        <v>36934</v>
+        <f t="shared" ref="M9:M14" si="10">SUM(K9:L9)</f>
+        <v>39745</v>
+      </c>
+      <c r="N9" s="3">
+        <v>24329</v>
+      </c>
+      <c r="O9" s="3">
+        <v>19440</v>
       </c>
       <c r="P9">
-        <f>SUM(P3:P8)</f>
-        <v>97134</v>
-      </c>
-      <c r="Q9">
-        <f>SUM(Q3:Q8)</f>
-        <v>74398</v>
-      </c>
-      <c r="R9">
-        <f>SUM(R3:R8)</f>
-        <v>45260</v>
+        <f>SUM(N9:O9)</f>
+        <v>43769</v>
+      </c>
+      <c r="Q9" s="3">
+        <v>27631</v>
+      </c>
+      <c r="R9" s="3">
+        <v>22334</v>
       </c>
       <c r="S9">
-        <f>SUM(S3:S8)</f>
-        <v>119658</v>
-      </c>
-      <c r="T9">
-        <f>SUM(T3:T8)</f>
-        <v>76055</v>
-      </c>
-      <c r="U9">
-        <f>SUM(U3:U8)</f>
-        <v>47649</v>
+        <f t="shared" ref="S9:S14" si="11">SUM(Q9:R9)</f>
+        <v>49965</v>
+      </c>
+      <c r="T9" s="3">
+        <v>27134</v>
+      </c>
+      <c r="U9" s="3">
+        <v>21771</v>
       </c>
       <c r="V9">
-        <f>SUM(V3:V8)</f>
-        <v>123704</v>
-      </c>
-      <c r="W9">
-        <f>SUM(W3:W8)</f>
-        <v>74274</v>
-      </c>
-      <c r="X9">
-        <f>SUM(X3:X8)</f>
-        <v>49100</v>
-      </c>
-      <c r="Y9">
-        <f>SUM(Y3:Y8)</f>
-        <v>123374</v>
-      </c>
-      <c r="Z9">
-        <f>SUM(Z3:Z8)</f>
-        <v>88299</v>
-      </c>
-      <c r="AA9">
-        <f>SUM(AA3:AA8)</f>
-        <v>61418</v>
-      </c>
-      <c r="AB9">
-        <f>SUM(AB3:AB8)</f>
-        <v>149717</v>
-      </c>
-      <c r="AC9">
-        <f>SUM(AC3:AC8)</f>
-        <v>98187</v>
-      </c>
-      <c r="AD9">
-        <f>SUM(AD3:AD8)</f>
-        <v>71305</v>
-      </c>
-      <c r="AE9">
-        <f>SUM(AE3:AE8)</f>
-        <v>169492</v>
-      </c>
-      <c r="AF9">
-        <f>SUM(AF3:AF8)</f>
-        <v>50415</v>
-      </c>
-      <c r="AG9">
-        <f>SUM(AG3:AG8)</f>
-        <v>38514</v>
-      </c>
-      <c r="AH9">
-        <f>SUM(AH3:AH8)</f>
-        <v>88929</v>
-      </c>
-      <c r="AI9">
-        <f>SUM(AI3:AI8)</f>
-        <v>41687</v>
-      </c>
-      <c r="AJ9">
-        <f>SUM(AJ3:AJ8)</f>
-        <v>28386</v>
-      </c>
-      <c r="AK9">
-        <f>SUM(AK3:AK8)</f>
-        <v>70073</v>
-      </c>
-      <c r="AL9">
-        <f>SUM(AL3:AL8)</f>
-        <v>53627</v>
-      </c>
-      <c r="AM9">
-        <f>SUM(AM3:AM8)</f>
-        <v>37323</v>
-      </c>
-      <c r="AN9">
-        <f>SUM(AN3:AN8)</f>
-        <v>90950</v>
-      </c>
-      <c r="AO9">
-        <f>SUM(AO3:AO8)</f>
-        <v>72029</v>
-      </c>
-      <c r="AP9">
-        <f>SUM(AP3:AP8)</f>
-        <v>53806</v>
-      </c>
-      <c r="AQ9">
-        <f>SUM(AQ3:AQ8)</f>
-        <v>125835</v>
-      </c>
-      <c r="AR9">
-        <f>SUM(AR3:AR8)</f>
-        <v>81155</v>
-      </c>
-      <c r="AS9">
-        <f>SUM(AS3:AS8)</f>
-        <v>61987</v>
-      </c>
-      <c r="AT9">
-        <f>SUM(AT3:AT8)</f>
-        <v>143142</v>
-      </c>
-      <c r="AU9">
-        <f>SUM(AU3:AU8)</f>
-        <v>80663</v>
-      </c>
-      <c r="AV9">
-        <f>SUM(AV3:AV8)</f>
-        <v>65113</v>
-      </c>
-      <c r="AW9">
-        <f>SUM(AW3:AW8)</f>
-        <v>145776</v>
-      </c>
-      <c r="AX9">
-        <f>SUM(AX3:AX8)</f>
-        <v>97442</v>
-      </c>
-      <c r="AY9">
-        <f>SUM(AY3:AY8)</f>
-        <v>77063</v>
-      </c>
-      <c r="AZ9">
-        <f>SUM(AZ3:AZ8)</f>
-        <v>174505</v>
+        <f>SUM(T9:U9)</f>
+        <v>48905</v>
+      </c>
+      <c r="W9" s="3">
+        <v>26492</v>
+      </c>
+      <c r="X9" s="3">
+        <v>22079</v>
+      </c>
+      <c r="Y9" s="3">
+        <v>48571</v>
+      </c>
+      <c r="Z9" s="3">
+        <v>30699</v>
+      </c>
+      <c r="AA9" s="3">
+        <v>27989</v>
+      </c>
+      <c r="AB9" s="3">
+        <v>58688</v>
+      </c>
+      <c r="AC9" s="3">
+        <v>33437</v>
+      </c>
+      <c r="AD9" s="3">
+        <v>31476</v>
+      </c>
+      <c r="AE9" s="3">
+        <v>64913</v>
+      </c>
+      <c r="AF9" s="3">
+        <v>22960</v>
+      </c>
+      <c r="AG9" s="3">
+        <v>21832</v>
+      </c>
+      <c r="AH9" s="3">
+        <v>44792</v>
+      </c>
+      <c r="AI9" s="3">
+        <v>21506</v>
+      </c>
+      <c r="AJ9" s="3">
+        <v>18968</v>
+      </c>
+      <c r="AK9" s="3">
+        <v>40474</v>
+      </c>
+      <c r="AL9" s="3">
+        <v>25903</v>
+      </c>
+      <c r="AM9" s="3">
+        <v>24138</v>
+      </c>
+      <c r="AN9" s="3">
+        <v>50041</v>
+      </c>
+      <c r="AO9" s="3">
+        <v>31040</v>
+      </c>
+      <c r="AP9" s="3">
+        <v>32117</v>
+      </c>
+      <c r="AQ9" s="3">
+        <v>63157</v>
+      </c>
+      <c r="AR9" s="3">
+        <v>42606</v>
+      </c>
+      <c r="AS9" s="3">
+        <v>42853</v>
+      </c>
+      <c r="AT9" s="3">
+        <v>85459</v>
+      </c>
+      <c r="AU9" s="3">
+        <v>39964</v>
+      </c>
+      <c r="AV9" s="3">
+        <v>41395</v>
+      </c>
+      <c r="AW9" s="3">
+        <v>81359</v>
+      </c>
+      <c r="AX9" s="3">
+        <v>46060</v>
+      </c>
+      <c r="AY9" s="3">
+        <v>49310</v>
+      </c>
+      <c r="AZ9" s="3">
+        <v>95370</v>
       </c>
     </row>
     <row r="10" spans="1:52" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10">
-        <f>B11-B9</f>
-        <v>89763</v>
-      </c>
-      <c r="C10">
-        <f t="shared" ref="C10:AZ10" si="7">C11-C9</f>
-        <v>88776</v>
+        <v>16</v>
+      </c>
+      <c r="B10" s="3">
+        <v>19296</v>
+      </c>
+      <c r="C10" s="3">
+        <v>18034</v>
       </c>
       <c r="D10">
         <f t="shared" si="7"/>
-        <v>178539</v>
-      </c>
-      <c r="E10">
-        <f t="shared" si="7"/>
-        <v>96139</v>
-      </c>
-      <c r="F10">
-        <f t="shared" si="7"/>
-        <v>93418</v>
+        <v>37330</v>
+      </c>
+      <c r="E10" s="3">
+        <v>21151</v>
+      </c>
+      <c r="F10" s="3">
+        <v>19424</v>
       </c>
       <c r="G10">
-        <f t="shared" si="7"/>
-        <v>189557</v>
-      </c>
-      <c r="H10">
-        <f t="shared" si="7"/>
-        <v>119059</v>
-      </c>
-      <c r="I10">
-        <f t="shared" si="7"/>
-        <v>109692</v>
+        <f t="shared" si="8"/>
+        <v>40575</v>
+      </c>
+      <c r="H10" s="3">
+        <v>23091</v>
+      </c>
+      <c r="I10" s="3">
+        <v>19828</v>
       </c>
       <c r="J10">
-        <f t="shared" si="7"/>
-        <v>228751</v>
-      </c>
-      <c r="K10">
-        <f t="shared" si="7"/>
-        <v>132366</v>
-      </c>
-      <c r="L10">
-        <f t="shared" si="7"/>
-        <v>120402</v>
+        <f t="shared" si="9"/>
+        <v>42919</v>
+      </c>
+      <c r="K10" s="3">
+        <v>27067</v>
+      </c>
+      <c r="L10" s="3">
+        <v>22669</v>
       </c>
       <c r="M10">
-        <f t="shared" si="7"/>
-        <v>252768</v>
-      </c>
-      <c r="N10">
-        <f t="shared" si="7"/>
-        <v>136008</v>
-      </c>
-      <c r="O10">
-        <f t="shared" si="7"/>
-        <v>121199</v>
+        <f t="shared" si="10"/>
+        <v>49736</v>
+      </c>
+      <c r="N10" s="3">
+        <v>28178</v>
+      </c>
+      <c r="O10" s="3">
+        <v>24232</v>
       </c>
       <c r="P10">
-        <f t="shared" si="7"/>
-        <v>257207</v>
-      </c>
-      <c r="Q10">
-        <f t="shared" si="7"/>
-        <v>154099</v>
-      </c>
-      <c r="R10">
-        <f t="shared" si="7"/>
-        <v>136829</v>
+        <f t="shared" ref="P10:P14" si="12">SUM(N10:O10)</f>
+        <v>52410</v>
+      </c>
+      <c r="Q10" s="3">
+        <v>31955</v>
+      </c>
+      <c r="R10" s="3">
+        <v>26890</v>
       </c>
       <c r="S10">
-        <f t="shared" si="7"/>
-        <v>290928</v>
-      </c>
-      <c r="T10">
-        <f t="shared" si="7"/>
-        <v>162764</v>
-      </c>
-      <c r="U10">
-        <f t="shared" si="7"/>
-        <v>145975</v>
+        <f t="shared" si="11"/>
+        <v>58845</v>
+      </c>
+      <c r="T10" s="3">
+        <v>31582</v>
+      </c>
+      <c r="U10" s="3">
+        <v>27166</v>
       </c>
       <c r="V10">
-        <f t="shared" si="7"/>
-        <v>308739</v>
-      </c>
-      <c r="W10">
-        <f t="shared" si="7"/>
-        <v>168707</v>
-      </c>
-      <c r="X10">
-        <f t="shared" si="7"/>
-        <v>153439</v>
-      </c>
-      <c r="Y10">
-        <f t="shared" si="7"/>
-        <v>322146</v>
-      </c>
-      <c r="Z10">
-        <f t="shared" si="7"/>
-        <v>170597</v>
-      </c>
-      <c r="AA10">
-        <f t="shared" si="7"/>
-        <v>161819</v>
-      </c>
-      <c r="AB10">
-        <f t="shared" si="7"/>
-        <v>332416</v>
-      </c>
-      <c r="AC10">
-        <f t="shared" si="7"/>
-        <v>180200</v>
-      </c>
-      <c r="AD10">
-        <f t="shared" si="7"/>
-        <v>171548</v>
-      </c>
-      <c r="AE10">
-        <f t="shared" si="7"/>
-        <v>351748</v>
-      </c>
-      <c r="AF10">
-        <f t="shared" si="7"/>
-        <v>248853</v>
-      </c>
-      <c r="AG10">
-        <f t="shared" si="7"/>
-        <v>233379</v>
-      </c>
-      <c r="AH10">
-        <f t="shared" si="7"/>
-        <v>482232</v>
-      </c>
-      <c r="AI10">
-        <f t="shared" si="7"/>
-        <v>273191</v>
-      </c>
-      <c r="AJ10">
-        <f t="shared" si="7"/>
-        <v>267237</v>
-      </c>
-      <c r="AK10">
-        <f t="shared" si="7"/>
-        <v>540428</v>
-      </c>
-      <c r="AL10">
-        <f t="shared" si="7"/>
-        <v>281150</v>
-      </c>
-      <c r="AM10">
-        <f t="shared" si="7"/>
-        <v>281687</v>
-      </c>
-      <c r="AN10">
-        <f t="shared" si="7"/>
-        <v>562837</v>
-      </c>
-      <c r="AO10">
-        <f t="shared" si="7"/>
-        <v>281832</v>
-      </c>
-      <c r="AP10">
-        <f t="shared" si="7"/>
-        <v>286103</v>
-      </c>
-      <c r="AQ10">
-        <f t="shared" si="7"/>
-        <v>567935</v>
-      </c>
-      <c r="AR10">
-        <f t="shared" si="7"/>
-        <v>297168</v>
-      </c>
-      <c r="AS10">
-        <f t="shared" si="7"/>
-        <v>302943</v>
-      </c>
-      <c r="AT10">
-        <f t="shared" si="7"/>
-        <v>600111</v>
-      </c>
-      <c r="AU10">
-        <f t="shared" si="7"/>
-        <v>338594</v>
-      </c>
-      <c r="AV10">
-        <f t="shared" si="7"/>
-        <v>338131</v>
-      </c>
-      <c r="AW10">
-        <f t="shared" si="7"/>
-        <v>676725</v>
-      </c>
-      <c r="AX10">
-        <f t="shared" si="7"/>
-        <v>344025</v>
-      </c>
-      <c r="AY10">
-        <f t="shared" si="7"/>
-        <v>358144</v>
-      </c>
-      <c r="AZ10">
-        <f t="shared" si="7"/>
-        <v>702169</v>
+        <f t="shared" ref="V10:V14" si="13">SUM(T10:U10)</f>
+        <v>58748</v>
+      </c>
+      <c r="W10" s="3">
+        <v>32385</v>
+      </c>
+      <c r="X10" s="3">
+        <v>28378</v>
+      </c>
+      <c r="Y10" s="3">
+        <v>60763</v>
+      </c>
+      <c r="Z10" s="3">
+        <v>36015</v>
+      </c>
+      <c r="AA10" s="3">
+        <v>34662</v>
+      </c>
+      <c r="AB10" s="3">
+        <v>70677</v>
+      </c>
+      <c r="AC10" s="3">
+        <v>37482</v>
+      </c>
+      <c r="AD10" s="3">
+        <v>36633</v>
+      </c>
+      <c r="AE10" s="3">
+        <v>74115</v>
+      </c>
+      <c r="AF10" s="3">
+        <v>30979</v>
+      </c>
+      <c r="AG10" s="3">
+        <v>30047</v>
+      </c>
+      <c r="AH10" s="3">
+        <v>61026</v>
+      </c>
+      <c r="AI10" s="3">
+        <v>31206</v>
+      </c>
+      <c r="AJ10" s="3">
+        <v>29834</v>
+      </c>
+      <c r="AK10" s="3">
+        <v>61040</v>
+      </c>
+      <c r="AL10" s="3">
+        <v>35700</v>
+      </c>
+      <c r="AM10" s="3">
+        <v>35729</v>
+      </c>
+      <c r="AN10" s="3">
+        <v>71429</v>
+      </c>
+      <c r="AO10" s="3">
+        <v>40323</v>
+      </c>
+      <c r="AP10" s="3">
+        <v>43112</v>
+      </c>
+      <c r="AQ10" s="3">
+        <v>83435</v>
+      </c>
+      <c r="AR10" s="3">
+        <v>54131</v>
+      </c>
+      <c r="AS10" s="3">
+        <v>55329</v>
+      </c>
+      <c r="AT10" s="3">
+        <v>109460</v>
+      </c>
+      <c r="AU10" s="3">
+        <v>48216</v>
+      </c>
+      <c r="AV10" s="3">
+        <v>51219</v>
+      </c>
+      <c r="AW10" s="3">
+        <v>99435</v>
+      </c>
+      <c r="AX10" s="3">
+        <v>56460</v>
+      </c>
+      <c r="AY10" s="3">
+        <v>62740</v>
+      </c>
+      <c r="AZ10" s="3">
+        <v>119200</v>
       </c>
     </row>
     <row r="11" spans="1:52" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11">
-        <v>128011</v>
-      </c>
-      <c r="C11">
-        <v>113632</v>
+        <v>17</v>
+      </c>
+      <c r="B11" s="3">
+        <v>20436</v>
+      </c>
+      <c r="C11" s="3">
+        <v>19785</v>
       </c>
       <c r="D11">
-        <v>241643</v>
-      </c>
-      <c r="E11">
-        <v>147400</v>
-      </c>
-      <c r="F11">
-        <v>124291</v>
+        <f t="shared" si="7"/>
+        <v>40221</v>
+      </c>
+      <c r="E11" s="3">
+        <v>21484</v>
+      </c>
+      <c r="F11" s="3">
+        <v>21504</v>
       </c>
       <c r="G11">
-        <v>271691</v>
-      </c>
-      <c r="H11">
-        <v>163369</v>
-      </c>
-      <c r="I11">
-        <v>138031</v>
+        <f t="shared" si="8"/>
+        <v>42988</v>
+      </c>
+      <c r="H11" s="3">
+        <v>25986</v>
+      </c>
+      <c r="I11" s="3">
+        <v>22967</v>
       </c>
       <c r="J11">
-        <v>301400</v>
-      </c>
-      <c r="K11">
-        <v>182475</v>
-      </c>
-      <c r="L11">
-        <v>151341</v>
+        <f t="shared" si="9"/>
+        <v>48953</v>
+      </c>
+      <c r="K11" s="3">
+        <v>30133</v>
+      </c>
+      <c r="L11" s="3">
+        <v>25943</v>
       </c>
       <c r="M11">
-        <v>333816</v>
-      </c>
-      <c r="N11">
-        <v>196208</v>
-      </c>
-      <c r="O11">
-        <v>158133</v>
+        <f t="shared" si="10"/>
+        <v>56076</v>
+      </c>
+      <c r="N11" s="3">
+        <v>30497</v>
+      </c>
+      <c r="O11" s="3">
+        <v>26265</v>
       </c>
       <c r="P11">
-        <v>354341</v>
-      </c>
-      <c r="Q11">
-        <v>228497</v>
-      </c>
-      <c r="R11">
-        <v>182089</v>
+        <f t="shared" si="12"/>
+        <v>56762</v>
+      </c>
+      <c r="Q11" s="3">
+        <v>34093</v>
+      </c>
+      <c r="R11" s="3">
+        <v>29760</v>
       </c>
       <c r="S11">
-        <v>410586</v>
-      </c>
-      <c r="T11">
-        <v>238819</v>
-      </c>
-      <c r="U11">
-        <v>193624</v>
+        <f t="shared" si="11"/>
+        <v>63853</v>
+      </c>
+      <c r="T11" s="3">
+        <v>35655</v>
+      </c>
+      <c r="U11" s="3">
+        <v>31548</v>
       </c>
       <c r="V11">
-        <v>432443</v>
-      </c>
-      <c r="W11">
-        <v>242981</v>
-      </c>
-      <c r="X11">
-        <v>202539</v>
-      </c>
-      <c r="Y11">
-        <v>445520</v>
-      </c>
-      <c r="Z11">
-        <v>258896</v>
-      </c>
-      <c r="AA11">
-        <v>223237</v>
-      </c>
-      <c r="AB11">
-        <v>482133</v>
-      </c>
-      <c r="AC11">
-        <v>278387</v>
-      </c>
-      <c r="AD11">
-        <v>242853</v>
-      </c>
-      <c r="AE11">
-        <v>521240</v>
-      </c>
-      <c r="AF11">
-        <v>299268</v>
-      </c>
-      <c r="AG11">
-        <v>271893</v>
-      </c>
-      <c r="AH11">
-        <v>571161</v>
-      </c>
-      <c r="AI11">
-        <v>314878</v>
-      </c>
-      <c r="AJ11">
-        <v>295623</v>
-      </c>
-      <c r="AK11">
-        <v>610501</v>
-      </c>
-      <c r="AL11">
-        <v>334777</v>
-      </c>
-      <c r="AM11">
-        <v>319010</v>
-      </c>
-      <c r="AN11">
-        <v>653787</v>
-      </c>
-      <c r="AO11">
-        <v>353861</v>
-      </c>
-      <c r="AP11">
-        <v>339909</v>
-      </c>
-      <c r="AQ11">
-        <v>693770</v>
-      </c>
-      <c r="AR11">
-        <v>378323</v>
-      </c>
-      <c r="AS11">
-        <v>364930</v>
-      </c>
-      <c r="AT11">
-        <v>743253</v>
-      </c>
-      <c r="AU11">
-        <v>419257</v>
-      </c>
-      <c r="AV11">
-        <v>403244</v>
-      </c>
-      <c r="AW11">
-        <v>822501</v>
-      </c>
-      <c r="AX11">
-        <v>441467</v>
-      </c>
-      <c r="AY11">
-        <v>435207</v>
-      </c>
-      <c r="AZ11">
-        <v>876674</v>
+        <f t="shared" si="13"/>
+        <v>67203</v>
+      </c>
+      <c r="W11" s="3">
+        <v>37703</v>
+      </c>
+      <c r="X11" s="3">
+        <v>34100</v>
+      </c>
+      <c r="Y11" s="3">
+        <v>71803</v>
+      </c>
+      <c r="Z11" s="3">
+        <v>38749</v>
+      </c>
+      <c r="AA11" s="3">
+        <v>37449</v>
+      </c>
+      <c r="AB11" s="3">
+        <v>76198</v>
+      </c>
+      <c r="AC11" s="3">
+        <v>40181</v>
+      </c>
+      <c r="AD11" s="3">
+        <v>38976</v>
+      </c>
+      <c r="AE11" s="3">
+        <v>79157</v>
+      </c>
+      <c r="AF11" s="3">
+        <v>41632</v>
+      </c>
+      <c r="AG11" s="3">
+        <v>39319</v>
+      </c>
+      <c r="AH11" s="3">
+        <v>80951</v>
+      </c>
+      <c r="AI11" s="3">
+        <v>45522</v>
+      </c>
+      <c r="AJ11" s="3">
+        <v>42925</v>
+      </c>
+      <c r="AK11" s="3">
+        <v>88447</v>
+      </c>
+      <c r="AL11" s="3">
+        <v>48628</v>
+      </c>
+      <c r="AM11" s="3">
+        <v>48237</v>
+      </c>
+      <c r="AN11" s="3">
+        <v>96865</v>
+      </c>
+      <c r="AO11" s="3">
+        <v>49930</v>
+      </c>
+      <c r="AP11" s="3">
+        <v>51863</v>
+      </c>
+      <c r="AQ11" s="3">
+        <v>101793</v>
+      </c>
+      <c r="AR11" s="3">
+        <v>59520</v>
+      </c>
+      <c r="AS11" s="3">
+        <v>58369</v>
+      </c>
+      <c r="AT11" s="3">
+        <v>117889</v>
+      </c>
+      <c r="AU11" s="3">
+        <v>57883</v>
+      </c>
+      <c r="AV11" s="3">
+        <v>58510</v>
+      </c>
+      <c r="AW11" s="3">
+        <v>116393</v>
+      </c>
+      <c r="AX11" s="3">
+        <v>64674</v>
+      </c>
+      <c r="AY11" s="3">
+        <v>70031</v>
+      </c>
+      <c r="AZ11" s="3">
+        <v>134705</v>
       </c>
     </row>
     <row r="12" spans="1:52" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12">
-        <f>100*(B9/B11)</f>
-        <v>29.878682300739779</v>
-      </c>
-      <c r="C12">
-        <f t="shared" ref="C12:AZ12" si="8">100*(C9/C11)</f>
-        <v>21.874119966206703</v>
+        <v>18</v>
+      </c>
+      <c r="B12" s="3">
+        <v>19144</v>
+      </c>
+      <c r="C12" s="3">
+        <v>19888</v>
       </c>
       <c r="D12">
-        <f t="shared" si="8"/>
-        <v>26.114557425623751</v>
-      </c>
-      <c r="E12">
-        <f t="shared" si="8"/>
-        <v>34.776797829036639</v>
-      </c>
-      <c r="F12">
-        <f t="shared" si="8"/>
-        <v>24.839288444054677</v>
+        <f t="shared" si="7"/>
+        <v>39032</v>
+      </c>
+      <c r="E12" s="3">
+        <v>20312</v>
+      </c>
+      <c r="F12" s="3">
+        <v>21435</v>
       </c>
       <c r="G12">
         <f t="shared" si="8"/>
+        <v>41747</v>
+      </c>
+      <c r="H12" s="3">
+        <v>27159</v>
+      </c>
+      <c r="I12" s="3">
+        <v>26449</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="9"/>
+        <v>53608</v>
+      </c>
+      <c r="K12" s="3">
+        <v>29846</v>
+      </c>
+      <c r="L12" s="3">
+        <v>29173</v>
+      </c>
+      <c r="M12">
+        <f t="shared" si="10"/>
+        <v>59019</v>
+      </c>
+      <c r="N12" s="3">
+        <v>29532</v>
+      </c>
+      <c r="O12" s="3">
+        <v>27329</v>
+      </c>
+      <c r="P12">
+        <f t="shared" si="12"/>
+        <v>56861</v>
+      </c>
+      <c r="Q12" s="3">
+        <v>32995</v>
+      </c>
+      <c r="R12" s="3">
+        <v>31397</v>
+      </c>
+      <c r="S12">
+        <f t="shared" si="11"/>
+        <v>64392</v>
+      </c>
+      <c r="T12" s="3">
+        <v>37694</v>
+      </c>
+      <c r="U12" s="3">
+        <v>35872</v>
+      </c>
+      <c r="V12">
+        <f t="shared" si="13"/>
+        <v>73566</v>
+      </c>
+      <c r="W12" s="3">
+        <v>39672</v>
+      </c>
+      <c r="X12" s="3">
+        <v>38505</v>
+      </c>
+      <c r="Y12" s="3">
+        <v>78177</v>
+      </c>
+      <c r="Z12" s="3">
+        <v>37365</v>
+      </c>
+      <c r="AA12" s="3">
+        <v>36136</v>
+      </c>
+      <c r="AB12" s="3">
+        <v>73501</v>
+      </c>
+      <c r="AC12" s="3">
+        <v>40442</v>
+      </c>
+      <c r="AD12" s="3">
+        <v>39113</v>
+      </c>
+      <c r="AE12" s="3">
+        <v>79555</v>
+      </c>
+      <c r="AF12" s="3">
+        <v>57487</v>
+      </c>
+      <c r="AG12" s="3">
+        <v>54648</v>
+      </c>
+      <c r="AH12" s="3">
+        <v>112135</v>
+      </c>
+      <c r="AI12" s="3">
+        <v>68572</v>
+      </c>
+      <c r="AJ12" s="3">
+        <v>66978</v>
+      </c>
+      <c r="AK12" s="3">
+        <v>135550</v>
+      </c>
+      <c r="AL12" s="3">
+        <v>72878</v>
+      </c>
+      <c r="AM12" s="3">
+        <v>75419</v>
+      </c>
+      <c r="AN12" s="3">
+        <v>148297</v>
+      </c>
+      <c r="AO12" s="3">
+        <v>67974</v>
+      </c>
+      <c r="AP12" s="3">
+        <v>69841</v>
+      </c>
+      <c r="AQ12" s="3">
+        <v>137815</v>
+      </c>
+      <c r="AR12" s="3">
+        <v>59130</v>
+      </c>
+      <c r="AS12" s="3">
+        <v>62800</v>
+      </c>
+      <c r="AT12" s="3">
+        <v>121930</v>
+      </c>
+      <c r="AU12" s="3">
+        <v>72069</v>
+      </c>
+      <c r="AV12" s="3">
+        <v>73925</v>
+      </c>
+      <c r="AW12" s="3">
+        <v>145994</v>
+      </c>
+      <c r="AX12" s="3">
+        <v>75429</v>
+      </c>
+      <c r="AY12" s="3">
+        <v>79605</v>
+      </c>
+      <c r="AZ12" s="3">
+        <v>155034</v>
+      </c>
+    </row>
+    <row r="13" spans="1:52" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="3">
+        <v>12615</v>
+      </c>
+      <c r="C13" s="3">
+        <v>14968</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="7"/>
+        <v>27583</v>
+      </c>
+      <c r="E13" s="3">
+        <v>11835</v>
+      </c>
+      <c r="F13" s="3">
+        <v>12632</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="8"/>
+        <v>24467</v>
+      </c>
+      <c r="H13" s="3">
+        <v>20395</v>
+      </c>
+      <c r="I13" s="3">
+        <v>21689</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="9"/>
+        <v>42084</v>
+      </c>
+      <c r="K13" s="3">
+        <v>19956</v>
+      </c>
+      <c r="L13" s="3">
+        <v>22318</v>
+      </c>
+      <c r="M13">
+        <f t="shared" si="10"/>
+        <v>42274</v>
+      </c>
+      <c r="N13" s="3">
+        <v>20245</v>
+      </c>
+      <c r="O13" s="3">
+        <v>20962</v>
+      </c>
+      <c r="P13">
+        <f>SUM(N13:O13)</f>
+        <v>41207</v>
+      </c>
+      <c r="Q13" s="3">
+        <v>23741</v>
+      </c>
+      <c r="R13" s="3">
+        <v>23532</v>
+      </c>
+      <c r="S13">
+        <f>SUM(Q13:R13)</f>
+        <v>47273</v>
+      </c>
+      <c r="T13" s="3">
+        <v>26436</v>
+      </c>
+      <c r="U13" s="3">
+        <v>25997</v>
+      </c>
+      <c r="V13">
+        <f t="shared" si="13"/>
+        <v>52433</v>
+      </c>
+      <c r="W13" s="3">
+        <v>28542</v>
+      </c>
+      <c r="X13" s="3">
+        <v>27251</v>
+      </c>
+      <c r="Y13" s="3">
+        <v>55793</v>
+      </c>
+      <c r="Z13" s="3">
+        <v>24542</v>
+      </c>
+      <c r="AA13" s="3">
+        <v>23174</v>
+      </c>
+      <c r="AB13" s="3">
+        <v>47716</v>
+      </c>
+      <c r="AC13" s="3">
+        <v>25531</v>
+      </c>
+      <c r="AD13" s="3">
+        <v>23127</v>
+      </c>
+      <c r="AE13" s="3">
+        <v>48658</v>
+      </c>
+      <c r="AF13" s="3">
+        <v>77718</v>
+      </c>
+      <c r="AG13" s="3">
+        <v>72211</v>
+      </c>
+      <c r="AH13" s="3">
+        <v>149929</v>
+      </c>
+      <c r="AI13" s="3">
+        <v>88040</v>
+      </c>
+      <c r="AJ13" s="3">
+        <v>91341</v>
+      </c>
+      <c r="AK13" s="3">
+        <v>179381</v>
+      </c>
+      <c r="AL13" s="3">
+        <v>81248</v>
+      </c>
+      <c r="AM13" s="3">
+        <v>84103</v>
+      </c>
+      <c r="AN13" s="3">
+        <v>165351</v>
+      </c>
+      <c r="AO13" s="3">
+        <v>76176</v>
+      </c>
+      <c r="AP13" s="3">
+        <v>76226</v>
+      </c>
+      <c r="AQ13" s="3">
+        <v>152402</v>
+      </c>
+      <c r="AR13" s="3">
+        <v>66563</v>
+      </c>
+      <c r="AS13" s="3">
+        <v>70780</v>
+      </c>
+      <c r="AT13" s="3">
+        <v>137343</v>
+      </c>
+      <c r="AU13" s="3">
+        <v>93851</v>
+      </c>
+      <c r="AV13" s="3">
+        <v>93495</v>
+      </c>
+      <c r="AW13" s="3">
+        <v>187346</v>
+      </c>
+      <c r="AX13" s="3">
+        <v>83503</v>
+      </c>
+      <c r="AY13" s="3">
+        <v>83819</v>
+      </c>
+      <c r="AZ13" s="3">
+        <v>167322</v>
+      </c>
+    </row>
+    <row r="14" spans="1:52" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="3">
+        <v>1822</v>
+      </c>
+      <c r="C14" s="3">
+        <v>1889</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="7"/>
+        <v>3711</v>
+      </c>
+      <c r="E14" s="3">
+        <v>1510</v>
+      </c>
+      <c r="F14" s="3">
+        <v>1442</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="8"/>
+        <v>2952</v>
+      </c>
+      <c r="H14" s="3">
+        <v>3665</v>
+      </c>
+      <c r="I14" s="3">
+        <v>3402</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="9"/>
+        <v>7067</v>
+      </c>
+      <c r="K14" s="3">
+        <v>3037</v>
+      </c>
+      <c r="L14" s="3">
+        <v>2881</v>
+      </c>
+      <c r="M14">
+        <f t="shared" si="10"/>
+        <v>5918</v>
+      </c>
+      <c r="N14" s="3">
+        <v>3227</v>
+      </c>
+      <c r="O14" s="3">
+        <v>2971</v>
+      </c>
+      <c r="P14">
+        <f t="shared" si="12"/>
+        <v>6198</v>
+      </c>
+      <c r="Q14" s="3">
+        <v>3684</v>
+      </c>
+      <c r="R14" s="3">
+        <v>2916</v>
+      </c>
+      <c r="S14">
+        <f t="shared" si="11"/>
+        <v>6600</v>
+      </c>
+      <c r="T14" s="3">
+        <v>4263</v>
+      </c>
+      <c r="U14" s="3">
+        <v>3621</v>
+      </c>
+      <c r="V14">
+        <f t="shared" si="13"/>
+        <v>7884</v>
+      </c>
+      <c r="W14" s="3">
+        <v>3913</v>
+      </c>
+      <c r="X14" s="3">
+        <v>3126</v>
+      </c>
+      <c r="Y14" s="3">
+        <v>7039</v>
+      </c>
+      <c r="Z14" s="3">
+        <v>3227</v>
+      </c>
+      <c r="AA14" s="3">
+        <v>2409</v>
+      </c>
+      <c r="AB14" s="3">
+        <v>5636</v>
+      </c>
+      <c r="AC14" s="3">
+        <v>3127</v>
+      </c>
+      <c r="AD14" s="3">
+        <v>2223</v>
+      </c>
+      <c r="AE14" s="3">
+        <v>5350</v>
+      </c>
+      <c r="AF14" s="3">
+        <v>18077</v>
+      </c>
+      <c r="AG14" s="3">
+        <v>15322</v>
+      </c>
+      <c r="AH14" s="3">
+        <v>33399</v>
+      </c>
+      <c r="AI14" s="3">
+        <v>18345</v>
+      </c>
+      <c r="AJ14" s="3">
+        <v>17191</v>
+      </c>
+      <c r="AK14" s="3">
+        <v>35536</v>
+      </c>
+      <c r="AL14" s="3">
+        <v>16793</v>
+      </c>
+      <c r="AM14" s="3">
+        <v>14061</v>
+      </c>
+      <c r="AN14" s="3">
+        <v>30854</v>
+      </c>
+      <c r="AO14" s="3">
+        <v>16389</v>
+      </c>
+      <c r="AP14" s="3">
+        <v>12944</v>
+      </c>
+      <c r="AQ14" s="3">
+        <v>29333</v>
+      </c>
+      <c r="AR14" s="3">
+        <v>15218</v>
+      </c>
+      <c r="AS14" s="3">
+        <v>12812</v>
+      </c>
+      <c r="AT14" s="3">
+        <v>28030</v>
+      </c>
+      <c r="AU14" s="3">
+        <v>26611</v>
+      </c>
+      <c r="AV14" s="3">
+        <v>19587</v>
+      </c>
+      <c r="AW14" s="3">
+        <v>46198</v>
+      </c>
+      <c r="AX14" s="3">
+        <v>17899</v>
+      </c>
+      <c r="AY14" s="3">
+        <v>12639</v>
+      </c>
+      <c r="AZ14" s="3">
+        <v>30538</v>
+      </c>
+    </row>
+    <row r="15" spans="1:52" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15">
+        <f>SUM(B3:B8)</f>
+        <v>38248</v>
+      </c>
+      <c r="C15">
+        <f>SUM(C3:C8)</f>
+        <v>24856</v>
+      </c>
+      <c r="D15">
+        <f>SUM(D3:D8)</f>
+        <v>63104</v>
+      </c>
+      <c r="E15">
+        <f>SUM(E3:E8)</f>
+        <v>51261</v>
+      </c>
+      <c r="F15">
+        <f>SUM(F3:F8)</f>
+        <v>30873</v>
+      </c>
+      <c r="G15">
+        <f>SUM(G3:G8)</f>
+        <v>82134</v>
+      </c>
+      <c r="H15">
+        <f>SUM(H3:H8)</f>
+        <v>44310</v>
+      </c>
+      <c r="I15">
+        <f>SUM(I3:I8)</f>
+        <v>28339</v>
+      </c>
+      <c r="J15">
+        <f>SUM(J3:J8)</f>
+        <v>72649</v>
+      </c>
+      <c r="K15">
+        <f>SUM(K3:K8)</f>
+        <v>50109</v>
+      </c>
+      <c r="L15">
+        <f>SUM(L3:L8)</f>
+        <v>30939</v>
+      </c>
+      <c r="M15">
+        <f>SUM(M3:M8)</f>
+        <v>81048</v>
+      </c>
+      <c r="N15">
+        <f>SUM(N3:N8)</f>
+        <v>60200</v>
+      </c>
+      <c r="O15">
+        <f>SUM(O3:O8)</f>
+        <v>36934</v>
+      </c>
+      <c r="P15">
+        <f>SUM(P3:P8)</f>
+        <v>97134</v>
+      </c>
+      <c r="Q15">
+        <f>SUM(Q3:Q8)</f>
+        <v>74398</v>
+      </c>
+      <c r="R15">
+        <f>SUM(R3:R8)</f>
+        <v>45260</v>
+      </c>
+      <c r="S15">
+        <f>SUM(S3:S8)</f>
+        <v>119658</v>
+      </c>
+      <c r="T15">
+        <f>SUM(T3:T8)</f>
+        <v>76055</v>
+      </c>
+      <c r="U15">
+        <f>SUM(U3:U8)</f>
+        <v>47649</v>
+      </c>
+      <c r="V15">
+        <f>SUM(V3:V8)</f>
+        <v>123704</v>
+      </c>
+      <c r="W15">
+        <f>SUM(W3:W8)</f>
+        <v>74274</v>
+      </c>
+      <c r="X15">
+        <f>SUM(X3:X8)</f>
+        <v>49100</v>
+      </c>
+      <c r="Y15">
+        <f>SUM(Y3:Y8)</f>
+        <v>123374</v>
+      </c>
+      <c r="Z15">
+        <f>SUM(Z3:Z8)</f>
+        <v>88299</v>
+      </c>
+      <c r="AA15">
+        <f>SUM(AA3:AA8)</f>
+        <v>61418</v>
+      </c>
+      <c r="AB15">
+        <f>SUM(AB3:AB8)</f>
+        <v>149717</v>
+      </c>
+      <c r="AC15">
+        <f>SUM(AC3:AC8)</f>
+        <v>98187</v>
+      </c>
+      <c r="AD15">
+        <f>SUM(AD3:AD8)</f>
+        <v>71305</v>
+      </c>
+      <c r="AE15">
+        <f>SUM(AE3:AE8)</f>
+        <v>169492</v>
+      </c>
+      <c r="AF15">
+        <f>SUM(AF3:AF8)</f>
+        <v>50415</v>
+      </c>
+      <c r="AG15">
+        <f>SUM(AG3:AG8)</f>
+        <v>38514</v>
+      </c>
+      <c r="AH15">
+        <f>SUM(AH3:AH8)</f>
+        <v>88929</v>
+      </c>
+      <c r="AI15">
+        <f>SUM(AI3:AI8)</f>
+        <v>41687</v>
+      </c>
+      <c r="AJ15">
+        <f>SUM(AJ3:AJ8)</f>
+        <v>28386</v>
+      </c>
+      <c r="AK15">
+        <f>SUM(AK3:AK8)</f>
+        <v>70073</v>
+      </c>
+      <c r="AL15">
+        <f>SUM(AL3:AL8)</f>
+        <v>53627</v>
+      </c>
+      <c r="AM15">
+        <f>SUM(AM3:AM8)</f>
+        <v>37323</v>
+      </c>
+      <c r="AN15">
+        <f>SUM(AN3:AN8)</f>
+        <v>90950</v>
+      </c>
+      <c r="AO15">
+        <f>SUM(AO3:AO8)</f>
+        <v>72029</v>
+      </c>
+      <c r="AP15">
+        <f>SUM(AP3:AP8)</f>
+        <v>53806</v>
+      </c>
+      <c r="AQ15">
+        <f>SUM(AQ3:AQ8)</f>
+        <v>125835</v>
+      </c>
+      <c r="AR15">
+        <f>SUM(AR3:AR8)</f>
+        <v>81155</v>
+      </c>
+      <c r="AS15">
+        <f>SUM(AS3:AS8)</f>
+        <v>61987</v>
+      </c>
+      <c r="AT15">
+        <f>SUM(AT3:AT8)</f>
+        <v>143142</v>
+      </c>
+      <c r="AU15">
+        <f>SUM(AU3:AU8)</f>
+        <v>80663</v>
+      </c>
+      <c r="AV15">
+        <f>SUM(AV3:AV8)</f>
+        <v>65113</v>
+      </c>
+      <c r="AW15">
+        <f>SUM(AW3:AW8)</f>
+        <v>145776</v>
+      </c>
+      <c r="AX15">
+        <f>SUM(AX3:AX8)</f>
+        <v>97442</v>
+      </c>
+      <c r="AY15">
+        <f>SUM(AY3:AY8)</f>
+        <v>77063</v>
+      </c>
+      <c r="AZ15">
+        <f>SUM(AZ3:AZ8)</f>
+        <v>174505</v>
+      </c>
+    </row>
+    <row r="16" spans="1:52" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="3">
+        <f>SUM(B9:B14)</f>
+        <v>89763</v>
+      </c>
+      <c r="C16" s="3">
+        <f t="shared" ref="C16:AZ16" si="14">SUM(C9:C14)</f>
+        <v>88776</v>
+      </c>
+      <c r="D16" s="3">
+        <f t="shared" si="14"/>
+        <v>178539</v>
+      </c>
+      <c r="E16" s="3">
+        <f t="shared" si="14"/>
+        <v>96139</v>
+      </c>
+      <c r="F16" s="3">
+        <f t="shared" si="14"/>
+        <v>93418</v>
+      </c>
+      <c r="G16" s="3">
+        <f t="shared" si="14"/>
+        <v>189557</v>
+      </c>
+      <c r="H16" s="3">
+        <f t="shared" si="14"/>
+        <v>119059</v>
+      </c>
+      <c r="I16" s="3">
+        <f t="shared" si="14"/>
+        <v>109692</v>
+      </c>
+      <c r="J16" s="3">
+        <f t="shared" si="14"/>
+        <v>228751</v>
+      </c>
+      <c r="K16" s="3">
+        <f t="shared" si="14"/>
+        <v>132366</v>
+      </c>
+      <c r="L16" s="3">
+        <f t="shared" si="14"/>
+        <v>120402</v>
+      </c>
+      <c r="M16" s="3">
+        <f t="shared" si="14"/>
+        <v>252768</v>
+      </c>
+      <c r="N16" s="3">
+        <f t="shared" si="14"/>
+        <v>136008</v>
+      </c>
+      <c r="O16" s="3">
+        <f t="shared" si="14"/>
+        <v>121199</v>
+      </c>
+      <c r="P16" s="3">
+        <f t="shared" si="14"/>
+        <v>257207</v>
+      </c>
+      <c r="Q16" s="3">
+        <f t="shared" si="14"/>
+        <v>154099</v>
+      </c>
+      <c r="R16" s="3">
+        <f t="shared" si="14"/>
+        <v>136829</v>
+      </c>
+      <c r="S16" s="3">
+        <f t="shared" si="14"/>
+        <v>290928</v>
+      </c>
+      <c r="T16" s="3">
+        <f t="shared" si="14"/>
+        <v>162764</v>
+      </c>
+      <c r="U16" s="3">
+        <f t="shared" si="14"/>
+        <v>145975</v>
+      </c>
+      <c r="V16" s="3">
+        <f t="shared" si="14"/>
+        <v>308739</v>
+      </c>
+      <c r="W16" s="3">
+        <f t="shared" si="14"/>
+        <v>168707</v>
+      </c>
+      <c r="X16" s="3">
+        <f t="shared" si="14"/>
+        <v>153439</v>
+      </c>
+      <c r="Y16" s="3">
+        <f t="shared" si="14"/>
+        <v>322146</v>
+      </c>
+      <c r="Z16" s="3">
+        <f t="shared" si="14"/>
+        <v>170597</v>
+      </c>
+      <c r="AA16" s="3">
+        <f t="shared" si="14"/>
+        <v>161819</v>
+      </c>
+      <c r="AB16" s="3">
+        <f t="shared" si="14"/>
+        <v>332416</v>
+      </c>
+      <c r="AC16" s="3">
+        <f t="shared" si="14"/>
+        <v>180200</v>
+      </c>
+      <c r="AD16" s="3">
+        <f t="shared" si="14"/>
+        <v>171548</v>
+      </c>
+      <c r="AE16" s="3">
+        <f t="shared" si="14"/>
+        <v>351748</v>
+      </c>
+      <c r="AF16" s="3">
+        <f t="shared" si="14"/>
+        <v>248853</v>
+      </c>
+      <c r="AG16" s="3">
+        <f t="shared" si="14"/>
+        <v>233379</v>
+      </c>
+      <c r="AH16" s="3">
+        <f t="shared" si="14"/>
+        <v>482232</v>
+      </c>
+      <c r="AI16" s="3">
+        <f t="shared" si="14"/>
+        <v>273191</v>
+      </c>
+      <c r="AJ16" s="3">
+        <f t="shared" si="14"/>
+        <v>267237</v>
+      </c>
+      <c r="AK16" s="3">
+        <f t="shared" si="14"/>
+        <v>540428</v>
+      </c>
+      <c r="AL16" s="3">
+        <f t="shared" si="14"/>
+        <v>281150</v>
+      </c>
+      <c r="AM16" s="3">
+        <f t="shared" si="14"/>
+        <v>281687</v>
+      </c>
+      <c r="AN16" s="3">
+        <f t="shared" si="14"/>
+        <v>562837</v>
+      </c>
+      <c r="AO16" s="3">
+        <f t="shared" si="14"/>
+        <v>281832</v>
+      </c>
+      <c r="AP16" s="3">
+        <f t="shared" si="14"/>
+        <v>286103</v>
+      </c>
+      <c r="AQ16" s="3">
+        <f t="shared" si="14"/>
+        <v>567935</v>
+      </c>
+      <c r="AR16" s="3">
+        <f t="shared" si="14"/>
+        <v>297168</v>
+      </c>
+      <c r="AS16" s="3">
+        <f t="shared" si="14"/>
+        <v>302943</v>
+      </c>
+      <c r="AT16" s="3">
+        <f t="shared" si="14"/>
+        <v>600111</v>
+      </c>
+      <c r="AU16" s="3">
+        <f t="shared" si="14"/>
+        <v>338594</v>
+      </c>
+      <c r="AV16" s="3">
+        <f t="shared" si="14"/>
+        <v>338131</v>
+      </c>
+      <c r="AW16" s="3">
+        <f t="shared" si="14"/>
+        <v>676725</v>
+      </c>
+      <c r="AX16" s="3">
+        <f t="shared" si="14"/>
+        <v>344025</v>
+      </c>
+      <c r="AY16" s="3">
+        <f t="shared" si="14"/>
+        <v>358144</v>
+      </c>
+      <c r="AZ16" s="3">
+        <f t="shared" si="14"/>
+        <v>702169</v>
+      </c>
+    </row>
+    <row r="17" spans="1:52" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17">
+        <v>128011</v>
+      </c>
+      <c r="C17">
+        <v>113632</v>
+      </c>
+      <c r="D17">
+        <v>241643</v>
+      </c>
+      <c r="E17">
+        <v>147400</v>
+      </c>
+      <c r="F17">
+        <v>124291</v>
+      </c>
+      <c r="G17">
+        <v>271691</v>
+      </c>
+      <c r="H17">
+        <v>163369</v>
+      </c>
+      <c r="I17">
+        <v>138031</v>
+      </c>
+      <c r="J17">
+        <v>301400</v>
+      </c>
+      <c r="K17">
+        <v>182475</v>
+      </c>
+      <c r="L17">
+        <v>151341</v>
+      </c>
+      <c r="M17">
+        <v>333816</v>
+      </c>
+      <c r="N17">
+        <v>196208</v>
+      </c>
+      <c r="O17">
+        <v>158133</v>
+      </c>
+      <c r="P17">
+        <v>354341</v>
+      </c>
+      <c r="Q17">
+        <v>228497</v>
+      </c>
+      <c r="R17">
+        <v>182089</v>
+      </c>
+      <c r="S17">
+        <v>410586</v>
+      </c>
+      <c r="T17">
+        <v>238819</v>
+      </c>
+      <c r="U17">
+        <v>193624</v>
+      </c>
+      <c r="V17">
+        <v>432443</v>
+      </c>
+      <c r="W17">
+        <v>242981</v>
+      </c>
+      <c r="X17">
+        <v>202539</v>
+      </c>
+      <c r="Y17">
+        <v>445520</v>
+      </c>
+      <c r="Z17">
+        <v>258896</v>
+      </c>
+      <c r="AA17">
+        <v>223237</v>
+      </c>
+      <c r="AB17">
+        <v>482133</v>
+      </c>
+      <c r="AC17">
+        <v>278387</v>
+      </c>
+      <c r="AD17">
+        <v>242853</v>
+      </c>
+      <c r="AE17">
+        <v>521240</v>
+      </c>
+      <c r="AF17">
+        <v>299268</v>
+      </c>
+      <c r="AG17">
+        <v>271893</v>
+      </c>
+      <c r="AH17">
+        <v>571161</v>
+      </c>
+      <c r="AI17">
+        <v>314878</v>
+      </c>
+      <c r="AJ17">
+        <v>295623</v>
+      </c>
+      <c r="AK17">
+        <v>610501</v>
+      </c>
+      <c r="AL17">
+        <v>334777</v>
+      </c>
+      <c r="AM17">
+        <v>319010</v>
+      </c>
+      <c r="AN17">
+        <v>653787</v>
+      </c>
+      <c r="AO17">
+        <v>353861</v>
+      </c>
+      <c r="AP17">
+        <v>339909</v>
+      </c>
+      <c r="AQ17">
+        <v>693770</v>
+      </c>
+      <c r="AR17">
+        <v>378323</v>
+      </c>
+      <c r="AS17">
+        <v>364930</v>
+      </c>
+      <c r="AT17">
+        <v>743253</v>
+      </c>
+      <c r="AU17">
+        <v>419257</v>
+      </c>
+      <c r="AV17">
+        <v>403244</v>
+      </c>
+      <c r="AW17">
+        <v>822501</v>
+      </c>
+      <c r="AX17">
+        <v>441467</v>
+      </c>
+      <c r="AY17">
+        <v>435207</v>
+      </c>
+      <c r="AZ17">
+        <v>876674</v>
+      </c>
+    </row>
+    <row r="18" spans="1:52" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18">
+        <f>100*(B15/B17)</f>
+        <v>29.878682300739779</v>
+      </c>
+      <c r="C18">
+        <f t="shared" ref="C18:AZ18" si="15">100*(C15/C17)</f>
+        <v>21.874119966206703</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="15"/>
+        <v>26.114557425623751</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="15"/>
+        <v>34.776797829036639</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="15"/>
+        <v>24.839288444054677</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="15"/>
         <v>30.230666455642623</v>
       </c>
-      <c r="H12">
-        <f t="shared" si="8"/>
+      <c r="H18">
+        <f t="shared" si="15"/>
         <v>27.122648727726801</v>
       </c>
-      <c r="I12">
-        <f t="shared" si="8"/>
+      <c r="I18">
+        <f t="shared" si="15"/>
         <v>20.530895233679392</v>
       </c>
-      <c r="J12">
-        <f t="shared" si="8"/>
+      <c r="J18">
+        <f t="shared" si="15"/>
         <v>24.103848706038487</v>
       </c>
-      <c r="K12">
-        <f t="shared" si="8"/>
+      <c r="K18">
+        <f t="shared" si="15"/>
         <v>27.460748047677765</v>
       </c>
-      <c r="L12">
-        <f t="shared" si="8"/>
+      <c r="L18">
+        <f t="shared" si="15"/>
         <v>20.443237457133229</v>
       </c>
-      <c r="M12">
-        <f t="shared" si="8"/>
+      <c r="M18">
+        <f t="shared" si="15"/>
         <v>24.279243655187287</v>
       </c>
-      <c r="N12">
-        <f t="shared" si="8"/>
+      <c r="N18">
+        <f t="shared" si="15"/>
         <v>30.681725515779174</v>
       </c>
-      <c r="O12">
-        <f t="shared" si="8"/>
+      <c r="O18">
+        <f t="shared" si="15"/>
         <v>23.356288693694548</v>
       </c>
-      <c r="P12">
-        <f t="shared" si="8"/>
+      <c r="P18">
+        <f t="shared" si="15"/>
         <v>27.412577150259214</v>
       </c>
-      <c r="Q12">
-        <f t="shared" si="8"/>
+      <c r="Q18">
+        <f t="shared" si="15"/>
         <v>32.559727261189423</v>
       </c>
-      <c r="R12">
-        <f t="shared" si="8"/>
+      <c r="R18">
+        <f t="shared" si="15"/>
         <v>24.855977022225396</v>
       </c>
-      <c r="S12">
-        <f t="shared" si="8"/>
+      <c r="S18">
+        <f t="shared" si="15"/>
         <v>29.143224561967529</v>
       </c>
-      <c r="T12">
-        <f t="shared" si="8"/>
+      <c r="T18">
+        <f t="shared" si="15"/>
         <v>31.846293636603452</v>
       </c>
-      <c r="U12">
-        <f t="shared" si="8"/>
+      <c r="U18">
+        <f t="shared" si="15"/>
         <v>24.609036069908687</v>
       </c>
-      <c r="V12">
-        <f t="shared" si="8"/>
+      <c r="V18">
+        <f t="shared" si="15"/>
         <v>28.605850944517542</v>
       </c>
-      <c r="W12">
-        <f t="shared" si="8"/>
+      <c r="W18">
+        <f t="shared" si="15"/>
         <v>30.567822175396429</v>
       </c>
-      <c r="X12">
-        <f t="shared" si="8"/>
+      <c r="X18">
+        <f t="shared" si="15"/>
         <v>24.242244703489206</v>
       </c>
-      <c r="Y12">
-        <f t="shared" si="8"/>
+      <c r="Y18">
+        <f t="shared" si="15"/>
         <v>27.692135033219607</v>
       </c>
-      <c r="Z12">
-        <f t="shared" si="8"/>
+      <c r="Z18">
+        <f t="shared" si="15"/>
         <v>34.105973054817376</v>
       </c>
-      <c r="AA12">
-        <f t="shared" si="8"/>
+      <c r="AA18">
+        <f t="shared" si="15"/>
         <v>27.512464331629616</v>
       </c>
-      <c r="AB12">
-        <f t="shared" si="8"/>
+      <c r="AB18">
+        <f t="shared" si="15"/>
         <v>31.05304967716377</v>
       </c>
-      <c r="AC12">
-        <f t="shared" si="8"/>
+      <c r="AC18">
+        <f t="shared" si="15"/>
         <v>35.269965910764512</v>
       </c>
-      <c r="AD12">
-        <f t="shared" si="8"/>
+      <c r="AD18">
+        <f t="shared" si="15"/>
         <v>29.361383223596167</v>
       </c>
-      <c r="AE12">
-        <f t="shared" si="8"/>
+      <c r="AE18">
+        <f t="shared" si="15"/>
         <v>32.517074668099148</v>
       </c>
-      <c r="AF12">
-        <f t="shared" si="8"/>
+      <c r="AF18">
+        <f t="shared" si="15"/>
         <v>16.846104494967719</v>
       </c>
-      <c r="AG12">
-        <f t="shared" si="8"/>
+      <c r="AG18">
+        <f t="shared" si="15"/>
         <v>14.165131136145471</v>
       </c>
-      <c r="AH12">
-        <f t="shared" si="8"/>
+      <c r="AH18">
+        <f t="shared" si="15"/>
         <v>15.569865589562312</v>
       </c>
-      <c r="AI12">
-        <f t="shared" si="8"/>
+      <c r="AI18">
+        <f t="shared" si="15"/>
         <v>13.239095776777038</v>
       </c>
-      <c r="AJ12">
-        <f t="shared" si="8"/>
+      <c r="AJ18">
+        <f t="shared" si="15"/>
         <v>9.6020945596249287</v>
       </c>
-      <c r="AK12">
-        <f t="shared" si="8"/>
+      <c r="AK18">
+        <f t="shared" si="15"/>
         <v>11.477950077067851</v>
       </c>
-      <c r="AL12">
-        <f t="shared" si="8"/>
+      <c r="AL18">
+        <f t="shared" si="15"/>
         <v>16.018722911072146</v>
       </c>
-      <c r="AM12">
-        <f t="shared" si="8"/>
+      <c r="AM18">
+        <f t="shared" si="15"/>
         <v>11.699633240337294</v>
       </c>
-      <c r="AN12">
-        <f t="shared" si="8"/>
+      <c r="AN18">
+        <f t="shared" si="15"/>
         <v>13.911258559744994</v>
       </c>
-      <c r="AO12">
-        <f t="shared" si="8"/>
+      <c r="AO18">
+        <f t="shared" si="15"/>
         <v>20.355167707094029</v>
       </c>
-      <c r="AP12">
-        <f t="shared" si="8"/>
+      <c r="AP18">
+        <f t="shared" si="15"/>
         <v>15.829530845020285</v>
       </c>
-      <c r="AQ12">
-        <f t="shared" si="8"/>
+      <c r="AQ18">
+        <f t="shared" si="15"/>
         <v>18.137855485247272</v>
       </c>
-      <c r="AR12">
-        <f t="shared" si="8"/>
+      <c r="AR18">
+        <f t="shared" si="15"/>
         <v>21.451246686032835</v>
       </c>
-      <c r="AS12">
-        <f t="shared" si="8"/>
+      <c r="AS18">
+        <f t="shared" si="15"/>
         <v>16.985997314553476</v>
       </c>
-      <c r="AT12">
-        <f t="shared" si="8"/>
+      <c r="AT18">
+        <f t="shared" si="15"/>
         <v>19.258852638334456</v>
       </c>
-      <c r="AU12">
-        <f t="shared" si="8"/>
+      <c r="AU18">
+        <f t="shared" si="15"/>
         <v>19.239511803022964</v>
       </c>
-      <c r="AV12">
-        <f t="shared" si="8"/>
+      <c r="AV18">
+        <f t="shared" si="15"/>
         <v>16.147295434030017</v>
       </c>
-      <c r="AW12">
-        <f t="shared" si="8"/>
+      <c r="AW18">
+        <f t="shared" si="15"/>
         <v>17.723504287532784</v>
       </c>
-      <c r="AX12">
-        <f t="shared" si="8"/>
+      <c r="AX18">
+        <f t="shared" si="15"/>
         <v>22.072317976202072</v>
       </c>
-      <c r="AY12">
-        <f t="shared" si="8"/>
+      <c r="AY18">
+        <f t="shared" si="15"/>
         <v>17.707205996227081</v>
       </c>
-      <c r="AZ12">
-        <f t="shared" si="8"/>
+      <c r="AZ18">
+        <f t="shared" si="15"/>
         <v>19.905346799380386</v>
       </c>
+    </row>
+    <row r="19" spans="1:52" x14ac:dyDescent="0.35">
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
+      <c r="J19" s="3"/>
+      <c r="K19" s="3"/>
+      <c r="L19" s="3"/>
+      <c r="M19" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>